<commit_message>
removing non-russian texts function added
</commit_message>
<xml_diff>
--- a/lemmatized_texts.xlsx
+++ b/lemmatized_texts.xlsx
@@ -921,11 +921,7 @@
       <c r="A50" t="n">
         <v>207391</v>
       </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>signature metsa noormees väga kaugel</t>
-        </is>
-      </c>
+      <c r="B50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">

</xml_diff>